<commit_message>
update rg+curseurs pour ssrha gme pypmsi
</commit_message>
<xml_diff>
--- a/formats/regpexpr/rg_curseurs.xlsx
+++ b/formats/regpexpr/rg_curseurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/regpexpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1B4A3C-FDD5-884B-A6DE-56B5003A650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB2C1D4-C59B-3A44-A4E5-1DD2031E536F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="27340" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="40">
   <si>
     <t>table</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>.{1,9}</t>
+  </si>
+  <si>
+    <t>ssrha_gme</t>
+  </si>
+  <si>
+    <t>zgme</t>
+  </si>
+  <si>
+    <t>.{1,13}</t>
+  </si>
+  <si>
+    <t>.{1,14}</t>
   </si>
 </sst>
 </file>
@@ -498,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181"/>
+    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3584,6 +3596,125 @@
       </c>
       <c r="E181">
         <v>17</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B182">
+        <v>2017</v>
+      </c>
+      <c r="C182" t="s">
+        <v>37</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E182">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B183">
+        <v>2018</v>
+      </c>
+      <c r="C183" t="s">
+        <v>37</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E183">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B184">
+        <v>2019</v>
+      </c>
+      <c r="C184" t="s">
+        <v>37</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E184">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B185">
+        <v>2020</v>
+      </c>
+      <c r="C185" t="s">
+        <v>37</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E185">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B186">
+        <v>2021</v>
+      </c>
+      <c r="C186" t="s">
+        <v>37</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E186">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B187">
+        <v>2022</v>
+      </c>
+      <c r="C187" t="s">
+        <v>37</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E187">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B188">
+        <v>2023</v>
+      </c>
+      <c r="C188" t="s">
+        <v>37</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E188">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include 2026 in inserts in .Rdata + regexp / curseurs
tested : it's ok.
waiting for druides
</commit_message>
<xml_diff>
--- a/formats/regpexpr/rg_curseurs.xlsx
+++ b/formats/regpexpr/rg_curseurs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/GitHub/formats_pmeasyr/formats/regpexpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD02A5-B38E-8248-8433-2B48DC8B7AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBA342B-E124-0148-9CD0-CE21274A90CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,24 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="40">
   <si>
     <t>table</t>
   </si>
@@ -148,11 +160,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,12 +208,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1356,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A181" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198:B206"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A193" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D213" sqref="D213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4869,6 +4888,159 @@
         <v>39</v>
       </c>
       <c r="E206" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B207" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E208" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E209" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B210" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E210" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B211" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E211" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B212" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E212" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B213" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E213" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B214" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E214" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B215" s="3">
+        <v>2026</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E215" s="3">
         <v>14</v>
       </c>
     </row>

</xml_diff>